<commit_message>
Added support for CHP + many fixes and updates
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigCY.xlsx
+++ b/ConfigFiles/ConfigCY.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="7425" windowHeight="1815"/>
@@ -11,12 +11,12 @@
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="ReserveParticipation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="153">
   <si>
     <t>Default value</t>
   </si>
@@ -309,9 +309,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>Database/PowerPlants/##/2015.csv</t>
-  </si>
-  <si>
     <t>Database/Load_RealTime/##/1h/2015.csv</t>
   </si>
   <si>
@@ -454,6 +451,30 @@
   </si>
   <si>
     <t>Simulations/simulationCY</t>
+  </si>
+  <si>
+    <t>Heat Demand</t>
+  </si>
+  <si>
+    <t>Database/Heat_demand/CY/Vassilikos_CCP2.csv</t>
+  </si>
+  <si>
+    <t>Price of Lignite</t>
+  </si>
+  <si>
+    <t>Price of Peat</t>
+  </si>
+  <si>
+    <t>CPLEX path</t>
+  </si>
+  <si>
+    <t>Database/PowerPlants/##/2015_heat.csv</t>
+  </si>
+  <si>
+    <t>Price of unserved heat</t>
+  </si>
+  <si>
+    <t>Load Shedding Cost</t>
   </si>
 </sst>
 </file>
@@ -542,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -603,9 +624,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -942,8 +960,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,16 +978,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -983,15 +1001,15 @@
     </row>
     <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
@@ -1007,15 +1025,15 @@
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="B6" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
@@ -1047,7 +1065,7 @@
         <v>39</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D18" s="14"/>
       <c r="H18" s="1" t="s">
@@ -1096,7 +1114,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>92</v>
       </c>
@@ -1107,7 +1125,18 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="24" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1169,7 @@
         <v>41</v>
       </c>
       <c r="C32" s="21">
-        <v>42369</v>
+        <v>42012</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>79</v>
@@ -1230,7 +1259,7 @@
     </row>
     <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>4</v>
@@ -1265,10 +1294,10 @@
       <c r="B62" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C62" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D62" s="23" t="s">
+      <c r="C62" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>96</v>
       </c>
       <c r="H62" s="12"/>
@@ -1280,8 +1309,8 @@
       <c r="B63" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="23" t="s">
+      <c r="C63" s="23"/>
+      <c r="D63" s="22" t="s">
         <v>96</v>
       </c>
       <c r="H63" s="12" t="s">
@@ -1295,14 +1324,14 @@
       <c r="B64" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C64" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D64" s="23" t="s">
+      <c r="C64" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="22" t="s">
         <v>96</v>
       </c>
       <c r="H64" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -1312,10 +1341,10 @@
       <c r="B65" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C65" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D65" s="23" t="s">
+      <c r="C65" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" s="22" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1326,8 +1355,8 @@
       <c r="B66" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C66" s="25"/>
-      <c r="D66" s="23" t="s">
+      <c r="C66" s="24"/>
+      <c r="D66" s="22" t="s">
         <v>96</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -1347,10 +1376,10 @@
       <c r="B67" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D67" s="23" t="s">
+      <c r="C67" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D67" s="22" t="s">
         <v>96</v>
       </c>
       <c r="H67" s="12" t="s">
@@ -1359,15 +1388,15 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C68" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D68" s="23" t="s">
+      <c r="C68" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D68" s="22" t="s">
         <v>96</v>
       </c>
       <c r="H68" s="12" t="s">
@@ -1376,13 +1405,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="25"/>
-      <c r="D69" s="23" t="s">
+      <c r="C69" s="24"/>
+      <c r="D69" s="22" t="s">
         <v>96</v>
       </c>
       <c r="H69" s="1" t="s">
@@ -1391,13 +1420,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C70" s="25"/>
-      <c r="D70" s="23"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="22"/>
       <c r="E70" s="1" t="s">
         <v>0</v>
       </c>
@@ -1407,13 +1436,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C71" s="25"/>
-      <c r="D71" s="23" t="s">
+      <c r="C71" s="24"/>
+      <c r="D71" s="22" t="s">
         <v>96</v>
       </c>
       <c r="E71" s="1" t="s">
@@ -1430,8 +1459,8 @@
       <c r="B72" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C72" s="25"/>
-      <c r="D72" s="23" t="s">
+      <c r="C72" s="24"/>
+      <c r="D72" s="22" t="s">
         <v>96</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -1441,7 +1470,7 @@
         <v>25</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -1451,10 +1480,10 @@
       <c r="B73" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C73" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D73" s="23" t="s">
+      <c r="C73" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D73" s="22" t="s">
         <v>96</v>
       </c>
       <c r="E73" s="1" t="s">
@@ -1466,15 +1495,15 @@
     </row>
     <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C74" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D74" s="23" t="s">
+      <c r="C74" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D74" s="22" t="s">
         <v>96</v>
       </c>
       <c r="E74" s="1" t="s">
@@ -1484,15 +1513,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C75" s="25"/>
-      <c r="D75" s="23" t="s">
+      <c r="C75" s="24"/>
+      <c r="D75" s="22" t="s">
         <v>96</v>
       </c>
       <c r="E75" s="1" t="s">
@@ -1502,29 +1531,109 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C76" s="25"/>
-      <c r="D76" s="23" t="s">
+      <c r="C76" s="24"/>
+      <c r="D76" s="22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="C77" s="22"/>
-    </row>
-    <row r="78" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C77" s="24"/>
+      <c r="D77" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D78" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F78" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C80" s="24"/>
+      <c r="D80" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F80" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" s="24"/>
+      <c r="D81" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F81" s="5">
+        <v>400</v>
+      </c>
+    </row>
     <row r="82" spans="1:6" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:6" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="C85" s="18"/>
@@ -1537,7 +1646,7 @@
       <c r="B87" s="6"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="30" t="s">
+      <c r="A88" s="29" t="s">
         <v>57</v>
       </c>
       <c r="B88" s="7" t="s">
@@ -1554,7 +1663,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
+      <c r="A89" s="29"/>
       <c r="B89" s="7" t="s">
         <v>5</v>
       </c>
@@ -1569,7 +1678,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="7" t="s">
         <v>6</v>
       </c>
@@ -1584,7 +1693,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
+      <c r="A91" s="29"/>
       <c r="B91" s="7" t="s">
         <v>33</v>
       </c>
@@ -1599,7 +1708,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="30"/>
+      <c r="A92" s="29"/>
       <c r="B92" s="7" t="s">
         <v>17</v>
       </c>
@@ -1614,7 +1723,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="29"/>
       <c r="B93" s="7" t="s">
         <v>7</v>
       </c>
@@ -1629,7 +1738,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="29"/>
       <c r="B94" s="7" t="s">
         <v>9</v>
       </c>
@@ -1644,7 +1753,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="7" t="s">
         <v>8</v>
       </c>
@@ -1659,7 +1768,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="30"/>
+      <c r="A96" s="29"/>
       <c r="B96" s="7" t="s">
         <v>10</v>
       </c>
@@ -1674,7 +1783,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="29"/>
       <c r="B97" s="7" t="s">
         <v>12</v>
       </c>
@@ -1689,7 +1798,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="30"/>
+      <c r="A98" s="29"/>
       <c r="B98" s="7" t="s">
         <v>13</v>
       </c>
@@ -1704,7 +1813,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="30"/>
+      <c r="A99" s="29"/>
       <c r="B99" s="7" t="s">
         <v>30</v>
       </c>
@@ -1719,7 +1828,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
+      <c r="A100" s="29"/>
       <c r="B100" s="7" t="s">
         <v>14</v>
       </c>
@@ -1734,7 +1843,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="29"/>
       <c r="B101" s="7" t="s">
         <v>15</v>
       </c>
@@ -1749,7 +1858,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
+      <c r="A102" s="29"/>
       <c r="B102" s="7" t="s">
         <v>21</v>
       </c>
@@ -1846,118 +1955,118 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B132" s="28" t="s">
+      <c r="B132" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C132" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B133" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C132" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B133" s="28" t="s">
+      <c r="C133" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B134" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C133" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B134" s="28" t="s">
+      <c r="C134" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B135" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C134" s="27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B135" s="28" t="s">
+      <c r="C135" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B136" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C135" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" s="28" t="s">
+      <c r="C136" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B137" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C136" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B137" s="28" t="s">
+      <c r="C137" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B138" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C137" s="27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="28" t="s">
+      <c r="C138" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B139" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="C138" s="27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B139" s="28" t="s">
+      <c r="C139" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B140" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C139" s="27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B140" s="28" t="s">
+      <c r="C140" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B141" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C140" s="27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="28" t="s">
+      <c r="C141" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B142" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="C141" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B142" s="28" t="s">
+      <c r="C142" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B143" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C142" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="28" t="s">
+      <c r="C143" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B144" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C143" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="28" t="s">
+      <c r="C144" s="26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C144" s="27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="C145" s="27" t="b">
+      <c r="C145" s="26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1971,7 +2080,7 @@
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B4:H4"/>
   </mergeCells>
-  <dataValidations count="13">
+  <dataValidations count="14">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C63"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C18:D18"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C31:D31">
@@ -1983,7 +2092,7 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C68"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F70:F74"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F70:F74 F77:F78 F80:F81"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C112"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C113"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C114"/>
@@ -1991,6 +2100,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C22"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F66"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F75"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C23"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2136,750 +2246,750 @@
   <sheetData>
     <row r="1" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="L1" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="20" t="s">
         <v>131</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" s="26" t="b">
+        <v>103</v>
+      </c>
+      <c r="B2" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" s="26" t="b">
+        <v>104</v>
+      </c>
+      <c r="B3" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="26" t="b">
+        <v>105</v>
+      </c>
+      <c r="B4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="26" t="b">
+        <v>106</v>
+      </c>
+      <c r="B5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" s="26" t="b">
+        <v>107</v>
+      </c>
+      <c r="B6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="25" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="26" t="b">
+        <v>108</v>
+      </c>
+      <c r="B7" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="26" t="b">
+        <v>109</v>
+      </c>
+      <c r="B8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="26" t="b">
+        <v>110</v>
+      </c>
+      <c r="B9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="26" t="b">
+        <v>111</v>
+      </c>
+      <c r="B10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="26" t="b">
+        <v>112</v>
+      </c>
+      <c r="B11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="26" t="b">
+        <v>113</v>
+      </c>
+      <c r="B12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="25" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" s="26" t="b">
+        <v>114</v>
+      </c>
+      <c r="B13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="25" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="26" t="b">
+        <v>115</v>
+      </c>
+      <c r="B14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="25" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" s="26" t="b">
+        <v>116</v>
+      </c>
+      <c r="B15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O16" s="26" t="b">
+        <v>117</v>
+      </c>
+      <c r="B16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="25" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated CHP and thermal storage formulation, added docs
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigCY.xlsx
+++ b/ConfigFiles/ConfigCY.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="7425" windowHeight="1815"/>
@@ -11,7 +11,7 @@
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="ReserveParticipation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -456,9 +456,6 @@
     <t>Heat Demand</t>
   </si>
   <si>
-    <t>Database/Heat_demand/CY/Vassilikos_CCP2.csv</t>
-  </si>
-  <si>
     <t>Price of Lignite</t>
   </si>
   <si>
@@ -468,13 +465,16 @@
     <t>CPLEX path</t>
   </si>
   <si>
-    <t>Database/PowerPlants/##/2015_heat.csv</t>
-  </si>
-  <si>
     <t>Price of unserved heat</t>
   </si>
   <si>
     <t>Load Shedding Cost</t>
+  </si>
+  <si>
+    <t>Database/PowerPlants/##/2015_heatpump.csv</t>
+  </si>
+  <si>
+    <t>Database/Heat_demand/CY/vassilikos_chp_p2h.csv</t>
   </si>
 </sst>
 </file>
@@ -961,14 +961,14 @@
   <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38" style="14" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" style="14" customWidth="1"/>
     <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>93</v>
@@ -1325,7 +1325,7 @@
         <v>39</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>96</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>39</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>39</v>
@@ -1589,7 +1589,7 @@
         <v>39</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D79" s="22" t="s">
         <v>96</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>39</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>39</v>

</xml_diff>